<commit_message>
adding accounts source file
</commit_message>
<xml_diff>
--- a/ft-a-04.xlsx
+++ b/ft-a-04.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/Library/Mobile Documents/com~apple~CloudDocs/Personal/Finances/Finance tracking/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jay/ftrack/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88F8FD9-D91D-0340-BAE1-521D572ACE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258D25CA-8AD1-504F-AA74-2634128A588D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107200" yWindow="-1100" windowWidth="38400" windowHeight="23500" activeTab="1" xr2:uid="{339D4989-ABBB-144A-8694-33787563D3BA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="16300" activeTab="1" xr2:uid="{339D4989-ABBB-144A-8694-33787563D3BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="49">
   <si>
     <t>Bernice Transactional</t>
   </si>
@@ -174,13 +174,16 @@
     <t>Bernice Credit Card</t>
   </si>
   <si>
-    <t>Home Repairs</t>
-  </si>
-  <si>
-    <t>Bernice Savings</t>
-  </si>
-  <si>
-    <t>Vehicel Savings</t>
+    <t>Jeanre Live Better</t>
+  </si>
+  <si>
+    <t>Bernice Live Better</t>
+  </si>
+  <si>
+    <t>Bernice Personal Savings</t>
+  </si>
+  <si>
+    <t>Home and Vehicle Savings</t>
   </si>
 </sst>
 </file>
@@ -967,114 +970,167 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A3564C-6FD2-944E-9DE9-C9098EF02BF5}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>1678993059</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>6002709354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>1706227645</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>6010640066</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>1421945264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>1817797296</v>
+      </c>
+      <c r="D7">
+        <v>1984239218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>1421952910</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>1759358744</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1434293481</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>1656301685</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>43</v>
       </c>
+      <c r="C12">
+        <v>1928213578</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13">
+        <v>1791077844</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>